<commit_message>
new manual, xlsx files and R files for manual
</commit_message>
<xml_diff>
--- a/inst/extdata/examples/xlsx/secondary-y-axis-not-auto.xlsx
+++ b/inst/extdata/examples/xlsx/secondary-y-axis-not-auto.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t xml:space="preserve">tab</t>
   </si>
@@ -67,6 +67,18 @@
   </si>
   <si>
     <t xml:space="preserve">n</t>
+  </si>
+  <si>
+    <t xml:space="preserve">x_date_format</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yyyy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">y_r_n_decimals</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1</t>
   </si>
   <si>
     <t xml:space="preserve">style</t>
@@ -509,7 +521,23 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="1"/>
+      <c r="A11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -527,13 +555,13 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B1" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="C1" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2">

</xml_diff>